<commit_message>
Change GUI, Password Show
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -906,12 +906,172 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1234567897</t>
-        </is>
+      <c r="G12" t="n">
+        <v>1234567897</v>
       </c>
       <c r="H12" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rohit Sharma</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>rohit@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Rohit45</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Rohit@987</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CEO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>7894561237</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Virat kohli</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>virat@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Virat18</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Virat@9876</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>4561237894</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Dhoni</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>dhoni@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Dhoni7</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Dhoni@987</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1234567891</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Csk</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Abhishek</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>abhi2@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Abhi456</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Abhi@987</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1234567891</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>

</xml_diff>

<commit_message>
Update Profile,Remove blank Window
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1745,10 +1745,8 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>1234567891</t>
-        </is>
+      <c r="F34" t="n">
+        <v>1234567891</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1758,6 +1756,168 @@
       <c r="H34" t="inlineStr">
         <is>
           <t>ravi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Akash Kawade</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Akash5880</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Akash@0992</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CEO</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>4567891231</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ozar</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>akash23@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tanmay</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Tanmay45</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Tanmay@987</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1234567897</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>tanmay@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Samarth</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Samarth18</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Samarth@987</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>4557896321</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>samarth1@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Rushi</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Rushi45</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Rushi@987</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>1234567898</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>pune</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>rushi@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>